<commit_message>
Improves readability and record collection
</commit_message>
<xml_diff>
--- a/seasons.xlsx
+++ b/seasons.xlsx
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1434" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1441" uniqueCount="36">
   <si>
     <t>L</t>
   </si>
@@ -4654,7 +4654,7 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4841,7 +4841,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14">
         <v>5</v>
@@ -4855,21 +4855,21 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16">
         <v>10</v>
@@ -4883,49 +4883,49 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18">
         <v>11</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B20">
         <v>6</v>
@@ -4939,99 +4939,127 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B21">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
       <c r="D21">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B22">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D22">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B23">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B24">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C24">
         <v>0</v>
       </c>
       <c r="D24">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B25">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C25">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B26">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C26">
         <v>0</v>
       </c>
       <c r="D26">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27">
+        <v>13</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>5</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B27">
-        <v>5</v>
-      </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-      <c r="D27">
+      <c r="B29">
+        <v>5</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
         <v>10</v>
       </c>
     </row>
@@ -5455,7 +5483,7 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>10</v>
@@ -5466,7 +5494,7 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -5480,7 +5508,7 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -5500,7 +5528,7 @@
         <v>1</v>
       </c>
       <c r="D5">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -5511,7 +5539,7 @@
         <v>6</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6">
         <v>9</v>
@@ -5522,7 +5550,7 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -5536,7 +5564,7 @@
         <v>29</v>
       </c>
       <c r="B8">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -5556,7 +5584,7 @@
         <v>1</v>
       </c>
       <c r="D9">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -5570,7 +5598,7 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -5584,7 +5612,7 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -5592,7 +5620,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -5609,7 +5637,7 @@
         <v>4</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13">
         <v>11</v>
@@ -5623,7 +5651,7 @@
         <v>6</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14">
         <v>9</v>
@@ -5637,7 +5665,7 @@
         <v>8</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15">
         <v>7</v>
@@ -5648,7 +5676,7 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -5665,7 +5693,7 @@
         <v>4</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17">
         <v>11</v>
@@ -5676,7 +5704,7 @@
         <v>18</v>
       </c>
       <c r="B18">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -5696,7 +5724,7 @@
         <v>1</v>
       </c>
       <c r="D19">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -5710,7 +5738,7 @@
         <v>0</v>
       </c>
       <c r="D20">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -5718,7 +5746,7 @@
         <v>21</v>
       </c>
       <c r="B21">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -5735,7 +5763,7 @@
         <v>9</v>
       </c>
       <c r="C22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D22">
         <v>4</v>
@@ -5749,7 +5777,7 @@
         <v>6</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23">
         <v>9</v>
@@ -5766,7 +5794,7 @@
         <v>0</v>
       </c>
       <c r="D24">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -5774,7 +5802,7 @@
         <v>25</v>
       </c>
       <c r="B25">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -5794,7 +5822,7 @@
         <v>0</v>
       </c>
       <c r="D26">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -5802,7 +5830,7 @@
         <v>30</v>
       </c>
       <c r="B27">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -5822,7 +5850,7 @@
         <v>0</v>
       </c>
       <c r="D28">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -5836,7 +5864,7 @@
         <v>0</v>
       </c>
       <c r="D29">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -8038,7 +8066,7 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -8169,83 +8197,83 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
         <v>13</v>
-      </c>
-      <c r="B12">
-        <v>8</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12">
-        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D14">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D15">
         <v>5</v>
@@ -8253,49 +8281,49 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="B17">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="B18">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C18">
         <v>0</v>
       </c>
       <c r="D18">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19">
         <v>8</v>
@@ -8309,7 +8337,7 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B20">
         <v>8</v>
@@ -8323,7 +8351,7 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B21">
         <v>8</v>
@@ -8337,13 +8365,13 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="1" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="B22">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D22">
         <v>8</v>
@@ -8351,127 +8379,141 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23">
         <v>7</v>
       </c>
       <c r="C23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D23">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D24">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B25">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D25">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="1" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B26">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C26">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D26">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C27">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D27">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B28">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D28">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B29">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D29">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B30">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C30">
         <v>0</v>
       </c>
       <c r="D30">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31">
+        <v>3</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B31">
-        <v>6</v>
-      </c>
-      <c r="C31">
-        <v>1</v>
-      </c>
-      <c r="D31">
+      <c r="B32">
+        <v>6</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
         <v>9</v>
       </c>
     </row>
@@ -8482,7 +8524,7 @@
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -8529,251 +8571,251 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D5">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="B7">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="B8">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D8">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D12">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D13">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D14">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D15">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
       <c r="D16">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="B17">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="B18">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19">
         <v>7</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B20">
         <v>7</v>
       </c>
       <c r="C20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D20">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B21">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D21">
         <v>7</v>
@@ -8781,141 +8823,155 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="1" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="B22">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D22">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D23">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B25">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C25">
         <v>0</v>
       </c>
       <c r="D25">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="1" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B26">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D26">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D27">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B28">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C28">
         <v>0</v>
       </c>
       <c r="D28">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B29">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D29">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B30">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C30">
         <v>1</v>
       </c>
       <c r="D30">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31">
+        <v>3</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B31">
-        <v>4</v>
-      </c>
-      <c r="C31">
-        <v>1</v>
-      </c>
-      <c r="D31">
+      <c r="B32">
+        <v>4</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
         <v>11</v>
       </c>
     </row>
@@ -8926,7 +8982,7 @@
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -9043,27 +9099,27 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9">
         <v>9</v>
       </c>
       <c r="C9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D9">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D10">
         <v>5</v>
@@ -9071,55 +9127,55 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11">
         <v>10</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12">
         <v>10</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14">
         <v>11</v>
@@ -9127,41 +9183,41 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D15">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D16">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="B17">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17">
         <v>6</v>
@@ -9169,139 +9225,139 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="B18">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C18">
         <v>0</v>
       </c>
       <c r="D18">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C19">
         <v>0</v>
       </c>
       <c r="D19">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B20">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C20">
         <v>0</v>
       </c>
       <c r="D20">
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B21">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C21">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="1" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="B22">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C22">
         <v>2</v>
       </c>
       <c r="D22">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23">
         <v>5</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D23">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
       <c r="D24">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B25">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D25">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="1" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B26">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D26">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D27">
         <v>7</v>
@@ -9309,57 +9365,71 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B28">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D28">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B29">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D29">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B30">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D30">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31">
+        <v>9</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B31">
-        <v>11</v>
-      </c>
-      <c r="C31">
-        <v>0</v>
-      </c>
-      <c r="D31">
+      <c r="B32">
+        <v>11</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
         <v>5</v>
       </c>
     </row>
@@ -17282,7 +17352,7 @@
 
 <file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -17385,153 +17455,153 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="B8">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D11">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D12">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B13">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
       <c r="D13">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B14">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
         <v>13</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15">
-        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="B16">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D16">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B18">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D18">
         <v>9</v>
@@ -17539,13 +17609,13 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B19">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C19">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D19">
         <v>4</v>
@@ -17553,169 +17623,197 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="B20">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C20">
         <v>0</v>
       </c>
       <c r="D20">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D21">
-        <v>13</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="1" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="B22">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C22">
         <v>0</v>
       </c>
       <c r="D22">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B23">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C23">
         <v>0</v>
       </c>
       <c r="D23">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="1" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="B24">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D24">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D25">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="1" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B26">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C26">
         <v>1</v>
       </c>
       <c r="D26">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B27">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D27">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C28">
         <v>1</v>
       </c>
       <c r="D28">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B29">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C29">
         <v>0</v>
       </c>
       <c r="D29">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B30">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C30">
         <v>1</v>
       </c>
       <c r="D30">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31">
+        <v>12</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32">
+        <v>7</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B31">
-        <v>3</v>
-      </c>
-      <c r="C31">
-        <v>0</v>
-      </c>
-      <c r="D31">
+      <c r="B33">
+        <v>3</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
         <v>13</v>
       </c>
     </row>

</xml_diff>